<commit_message>
Fix a couple of formatting errors in the standardized xlsx
</commit_message>
<xml_diff>
--- a/supplemental_data/data_sources_standardized.xlsx
+++ b/supplemental_data/data_sources_standardized.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Keith/Dev/research/johns-hopkins/dredze/mental-health-datasets/supplemental_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB02A1FC-C835-F94E-893D-1504FAF8A3DB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200B73E1-9814-6E4C-9A89-590F04E628E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="26060" windowHeight="11880" xr2:uid="{A1A2B0B9-EC2A-0C4B-9F85-EE07A9280363}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="26060" windowHeight="11880" xr2:uid="{A1A2B0B9-EC2A-0C4B-9F85-EE07A9280363}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="785" uniqueCount="398">
   <si>
     <t>title</t>
   </si>
@@ -255,9 +255,6 @@
     <t>De Choudhury, Gamon, Counts, Horvitz</t>
   </si>
   <si>
-    <t>depression_(476)</t>
-  </si>
-  <si>
     <t>https://www.aaai.org/ocs/index.php/ICWSM/ICWSM13/paper/viewFile/6124/6351</t>
   </si>
   <si>
@@ -270,9 +267,6 @@
     <t>survey_(personality)</t>
   </si>
   <si>
-    <t>depression_(28.4k)</t>
-  </si>
-  <si>
     <t>no_longer_exists</t>
   </si>
   <si>
@@ -672,9 +666,6 @@
     <t>survey_(clinical), interview</t>
   </si>
   <si>
-    <t>combined (&gt;1000k)</t>
-  </si>
-  <si>
     <t>https://www.ncbi.nlm.nih.gov/pmc/articles/PMC6442737/</t>
   </si>
   <si>
@@ -1222,6 +1213,18 @@
   </si>
   <si>
     <t>depression (53), control (101)</t>
+  </si>
+  <si>
+    <t>combined (1000k)</t>
+  </si>
+  <si>
+    <t>depression (476)</t>
+  </si>
+  <si>
+    <t>depression (28.4k)</t>
+  </si>
+  <si>
+    <t>combined (253)</t>
   </si>
 </sst>
 </file>
@@ -1589,8 +1592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F7582B-A8CE-1545-B88D-1FB6E3E8BB38}">
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="F70" sqref="F70"/>
+    <sheetView tabSelected="1" topLeftCell="G57" workbookViewId="0">
+      <selection activeCell="N59" sqref="N59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1812,8 +1815,8 @@
       <c r="J5" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="K5" s="1">
-        <v>253</v>
+      <c r="K5" s="1" t="s">
+        <v>397</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>23</v>
@@ -2021,7 +2024,7 @@
         <v>21</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>74</v>
+        <v>395</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>41</v>
@@ -2033,7 +2036,7 @@
         <v>9</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -2041,10 +2044,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="D11" s="1">
         <v>2014</v>
@@ -2056,19 +2059,19 @@
         <v>53</v>
       </c>
       <c r="G11" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L11" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>80</v>
       </c>
       <c r="M11" s="1" t="s">
         <v>23</v>
@@ -2077,7 +2080,7 @@
         <v>10</v>
       </c>
       <c r="O11" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -2085,10 +2088,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D12" s="1">
         <v>2015</v>
@@ -2106,19 +2109,19 @@
         <v>21</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="K12" s="1" t="s">
         <v>41</v>
       </c>
       <c r="M12" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="N12" s="1">
         <v>11</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -2126,10 +2129,10 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D13" s="1">
         <v>2016</v>
@@ -2147,7 +2150,7 @@
         <v>21</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="K13" s="1" t="s">
         <v>41</v>
@@ -2162,7 +2165,7 @@
         <v>12</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -2170,10 +2173,10 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D14" s="1">
         <v>2014</v>
@@ -2182,7 +2185,7 @@
         <v>3</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>20</v>
@@ -2191,7 +2194,7 @@
         <v>21</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K14" s="1" t="s">
         <v>41</v>
@@ -2206,7 +2209,7 @@
         <v>13</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -2214,10 +2217,10 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D15" s="1">
         <v>2015</v>
@@ -2235,10 +2238,10 @@
         <v>21</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K15" s="1" t="s">
         <v>41</v>
@@ -2253,7 +2256,7 @@
         <v>2</v>
       </c>
       <c r="O15" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -2261,10 +2264,10 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D16" s="1">
         <v>2016</v>
@@ -2273,7 +2276,7 @@
         <v>3</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>54</v>
@@ -2282,7 +2285,7 @@
         <v>21</v>
       </c>
       <c r="I16" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K16" s="1" t="s">
         <v>41</v>
@@ -2297,7 +2300,7 @@
         <v>15</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="34" x14ac:dyDescent="0.2">
@@ -2305,10 +2308,10 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D17" s="1">
         <v>2017</v>
@@ -2341,7 +2344,7 @@
         <v>1</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="170" x14ac:dyDescent="0.2">
@@ -2349,10 +2352,10 @@
         <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D18" s="2">
         <v>2016</v>
@@ -2361,19 +2364,19 @@
         <v>5</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L18" s="1" t="s">
         <v>111</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="M18" s="1" t="s">
         <v>23</v>
@@ -2382,7 +2385,7 @@
         <v>17</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="102" x14ac:dyDescent="0.2">
@@ -2390,10 +2393,10 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D19" s="1">
         <v>2016</v>
@@ -2402,22 +2405,22 @@
         <v>5</v>
       </c>
       <c r="F19" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>119</v>
-      </c>
       <c r="H19" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I19" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="K19" s="1" t="s">
         <v>41</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M19" s="1" t="s">
         <v>23</v>
@@ -2426,7 +2429,7 @@
         <v>18</v>
       </c>
       <c r="O19" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -2434,10 +2437,10 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D20" s="1">
         <v>2017</v>
@@ -2446,25 +2449,25 @@
         <v>5</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="K20" s="1" t="s">
         <v>41</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M20" s="1" t="s">
         <v>23</v>
@@ -2473,7 +2476,7 @@
         <v>19</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -2481,31 +2484,31 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D21" s="1">
         <v>2016</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="H21" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>134</v>
       </c>
       <c r="K21" s="1" t="s">
         <v>41</v>
@@ -2517,7 +2520,7 @@
         <v>20</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -2525,10 +2528,10 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D22" s="1">
         <v>2015</v>
@@ -2537,7 +2540,7 @@
         <v>3</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>54</v>
@@ -2549,7 +2552,7 @@
         <v>41</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K22" s="1" t="s">
         <v>41</v>
@@ -2564,7 +2567,7 @@
         <v>21</v>
       </c>
       <c r="O22" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -2572,10 +2575,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D23" s="1">
         <v>2013</v>
@@ -2593,19 +2596,19 @@
         <v>21</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="K23" s="1" t="s">
         <v>41</v>
       </c>
       <c r="M23" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="N23" s="1">
         <v>22</v>
       </c>
       <c r="O23" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -2613,10 +2616,10 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D24" s="1">
         <v>2018</v>
@@ -2628,19 +2631,19 @@
         <v>53</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="K24" s="1" t="s">
         <v>41</v>
       </c>
       <c r="L24" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M24" s="1" t="s">
         <v>23</v>
@@ -2649,7 +2652,7 @@
         <v>23</v>
       </c>
       <c r="O24" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="85" x14ac:dyDescent="0.2">
@@ -2657,10 +2660,10 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D25" s="1">
         <v>2017</v>
@@ -2669,7 +2672,7 @@
         <v>3</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="G25" s="1" t="s">
         <v>20</v>
@@ -2678,10 +2681,10 @@
         <v>21</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="K25" s="1" t="s">
         <v>41</v>
@@ -2693,10 +2696,10 @@
         <v>23</v>
       </c>
       <c r="N25" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="O25" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -2704,10 +2707,10 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D26" s="1">
         <v>2018</v>
@@ -2716,22 +2719,22 @@
         <v>5</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I26" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="K26" s="1" t="s">
         <v>41</v>
       </c>
       <c r="L26" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M26" s="1" t="s">
         <v>23</v>
@@ -2740,7 +2743,7 @@
         <v>25</v>
       </c>
       <c r="O26" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="85" x14ac:dyDescent="0.2">
@@ -2748,28 +2751,28 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D27" s="1">
         <v>2015</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>21</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K27" s="1" t="s">
         <v>41</v>
@@ -2784,7 +2787,7 @@
         <v>26</v>
       </c>
       <c r="O27" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -2792,10 +2795,10 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D28" s="1">
         <v>2017</v>
@@ -2828,7 +2831,7 @@
         <v>1</v>
       </c>
       <c r="O28" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="102" x14ac:dyDescent="0.2">
@@ -2836,37 +2839,37 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D29" s="1">
         <v>2018</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F29" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I29" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K29" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L29" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="K29" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L29" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="M29" s="1" t="s">
         <v>23</v>
@@ -2875,7 +2878,7 @@
         <v>28</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="85" x14ac:dyDescent="0.2">
@@ -2883,28 +2886,28 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D30" s="1">
         <v>2019</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F30" s="1" t="s">
         <v>41</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>21</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="K30" s="1" t="s">
         <v>41</v>
@@ -2919,7 +2922,7 @@
         <v>26</v>
       </c>
       <c r="O30" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="85" x14ac:dyDescent="0.2">
@@ -2927,16 +2930,16 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D31" s="1">
         <v>2014</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F31" s="1" t="s">
         <v>53</v>
@@ -2948,7 +2951,7 @@
         <v>21</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M31" s="1" t="s">
         <v>23</v>
@@ -2957,7 +2960,7 @@
         <v>30</v>
       </c>
       <c r="O31" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="32" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -2965,28 +2968,28 @@
         <v>31</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D32" s="1">
         <v>2016</v>
       </c>
       <c r="E32" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="G32" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="F32" s="1" t="s">
-        <v>189</v>
-      </c>
-      <c r="G32" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="K32" s="1" t="s">
         <v>41</v>
@@ -3001,7 +3004,7 @@
         <v>31</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -3009,19 +3012,19 @@
         <v>32</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D33" s="1">
         <v>2018</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>54</v>
@@ -3030,19 +3033,19 @@
         <v>55</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K33" s="1" t="s">
         <v>41</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="N33" s="1">
         <v>32</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="34" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -3050,19 +3053,19 @@
         <v>33</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D34" s="1">
         <v>2019</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="G34" s="1" t="s">
         <v>48</v>
@@ -3071,7 +3074,7 @@
         <v>21</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>41</v>
@@ -3083,7 +3086,7 @@
         <v>33</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="35" spans="1:15" ht="372" x14ac:dyDescent="0.2">
@@ -3091,10 +3094,10 @@
         <v>34</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D35" s="1">
         <v>2018</v>
@@ -3103,16 +3106,16 @@
         <v>5</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="K35" s="1" t="s">
         <v>41</v>
@@ -3127,7 +3130,7 @@
         <v>34</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="36" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -3135,37 +3138,37 @@
         <v>35</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D36" s="1">
         <v>2018</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I36" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="K36" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L36" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="J36" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="K36" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="L36" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="M36" s="1" t="s">
         <v>23</v>
@@ -3174,7 +3177,7 @@
         <v>28</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="37" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -3182,10 +3185,10 @@
         <v>36</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D37" s="1">
         <v>2017</v>
@@ -3203,7 +3206,7 @@
         <v>21</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K37" s="1" t="s">
         <v>41</v>
@@ -3218,7 +3221,7 @@
         <v>36</v>
       </c>
       <c r="O37" s="1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:15" ht="85" x14ac:dyDescent="0.2">
@@ -3226,10 +3229,10 @@
         <v>37</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D38" s="1">
         <v>2017</v>
@@ -3238,7 +3241,7 @@
         <v>3</v>
       </c>
       <c r="F38" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G38" s="1" t="s">
         <v>54</v>
@@ -3259,7 +3262,7 @@
         <v>37</v>
       </c>
       <c r="O38" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="39" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -3267,10 +3270,10 @@
         <v>38</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="D39" s="1">
         <v>2019</v>
@@ -3279,7 +3282,7 @@
         <v>5</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>54</v>
@@ -3288,10 +3291,10 @@
         <v>21</v>
       </c>
       <c r="I39" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="K39" s="1" t="s">
         <v>41</v>
@@ -3306,7 +3309,7 @@
         <v>38</v>
       </c>
       <c r="O39" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="170" x14ac:dyDescent="0.2">
@@ -3314,10 +3317,10 @@
         <v>39</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="D40" s="1">
         <v>2016</v>
@@ -3329,19 +3332,19 @@
         <v>53</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>55</v>
       </c>
       <c r="J40" s="1" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>41</v>
       </c>
       <c r="L40" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="M40" s="1" t="s">
         <v>23</v>
@@ -3350,7 +3353,7 @@
         <v>39</v>
       </c>
       <c r="O40" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="41" spans="1:15" ht="85" x14ac:dyDescent="0.2">
@@ -3358,28 +3361,28 @@
         <v>40</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="D41" s="1">
         <v>2019</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="K41" s="1" t="s">
         <v>41</v>
@@ -3394,7 +3397,7 @@
         <v>40</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="42" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -3402,10 +3405,10 @@
         <v>41</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D42" s="1">
         <v>2015</v>
@@ -3414,22 +3417,22 @@
         <v>3</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>55</v>
       </c>
       <c r="J42" s="1" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="K42" s="1" t="s">
         <v>41</v>
       </c>
       <c r="L42" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="M42" s="1" t="s">
         <v>23</v>
@@ -3438,7 +3441,7 @@
         <v>41</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="43" spans="1:15" ht="119" x14ac:dyDescent="0.2">
@@ -3446,10 +3449,10 @@
         <v>42</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="D43" s="1">
         <v>2018</v>
@@ -3458,7 +3461,7 @@
         <v>5</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="G43" s="1" t="s">
         <v>20</v>
@@ -3467,7 +3470,7 @@
         <v>21</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="K43" s="1" t="s">
         <v>41</v>
@@ -3482,7 +3485,7 @@
         <v>42</v>
       </c>
       <c r="O43" s="1" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="44" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -3490,10 +3493,10 @@
         <v>43</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
       <c r="D44" s="1">
         <v>2018</v>
@@ -3502,16 +3505,16 @@
         <v>5</v>
       </c>
       <c r="F44" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>55</v>
       </c>
       <c r="J44" s="1" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="K44" s="1" t="s">
         <v>41</v>
@@ -3526,7 +3529,7 @@
         <v>43</v>
       </c>
       <c r="O44" s="1" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="45" spans="1:15" ht="85" x14ac:dyDescent="0.2">
@@ -3534,10 +3537,10 @@
         <v>44</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D45" s="1">
         <v>2015</v>
@@ -3549,19 +3552,19 @@
         <v>53</v>
       </c>
       <c r="G45" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>55</v>
       </c>
       <c r="J45" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="K45" s="1" t="s">
         <v>41</v>
       </c>
       <c r="L45" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="M45" s="1" t="s">
         <v>23</v>
@@ -3570,7 +3573,7 @@
         <v>44</v>
       </c>
       <c r="O45" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="46" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -3578,28 +3581,28 @@
         <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D46" s="1">
         <v>2019</v>
       </c>
       <c r="E46" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="F46" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="K46" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="G46" s="1" t="s">
-        <v>190</v>
-      </c>
-      <c r="H46" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="K46" s="1" t="s">
-        <v>265</v>
       </c>
       <c r="M46" s="1" t="s">
         <v>23</v>
@@ -3608,7 +3611,7 @@
         <v>45</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="47" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -3616,37 +3619,37 @@
         <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="D47" s="1">
         <v>2015</v>
       </c>
       <c r="E47" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="F47" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I47" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="J47" s="1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="K47" s="1" t="s">
         <v>41</v>
       </c>
       <c r="L47" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M47" s="1" t="s">
         <v>23</v>
@@ -3655,7 +3658,7 @@
         <v>46</v>
       </c>
       <c r="O47" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="48" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -3663,19 +3666,19 @@
         <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="D48" s="1">
         <v>2014</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F48" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G48" s="1" t="s">
         <v>48</v>
@@ -3684,19 +3687,19 @@
         <v>21</v>
       </c>
       <c r="I48" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="K48" s="1" t="s">
         <v>41</v>
       </c>
       <c r="M48" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="N48" s="1">
         <v>47</v>
       </c>
       <c r="O48" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="102" x14ac:dyDescent="0.2">
@@ -3704,19 +3707,19 @@
         <v>48</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="D49" s="1">
         <v>2015</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>48</v>
@@ -3725,19 +3728,19 @@
         <v>21</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="K49" s="1" t="s">
         <v>41</v>
       </c>
       <c r="M49" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="N49" s="1">
         <v>48</v>
       </c>
       <c r="O49" s="1" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -3745,43 +3748,43 @@
         <v>49</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="D50" s="1">
         <v>2014</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="J50" s="1" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="K50" s="1" t="s">
         <v>41</v>
       </c>
       <c r="M50" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="N50" s="1">
         <v>47</v>
       </c>
       <c r="O50" s="1" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="85" x14ac:dyDescent="0.2">
@@ -3789,28 +3792,28 @@
         <v>50</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="D51" s="1">
         <v>2019</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H51" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="I51" s="1" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="K51" s="1" t="s">
         <v>41</v>
@@ -3822,7 +3825,7 @@
         <v>50</v>
       </c>
       <c r="O51" s="3" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="102" x14ac:dyDescent="0.2">
@@ -3830,10 +3833,10 @@
         <v>51</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="D52" s="1">
         <v>2017</v>
@@ -3842,25 +3845,25 @@
         <v>5</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I52" s="1" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="J52" s="1" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="K52" s="1" t="s">
         <v>41</v>
       </c>
       <c r="L52" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M52" s="1" t="s">
         <v>23</v>
@@ -3869,7 +3872,7 @@
         <v>51</v>
       </c>
       <c r="O52" s="1" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
     </row>
     <row r="53" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -3877,10 +3880,10 @@
         <v>52</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="D53" s="1">
         <v>2019</v>
@@ -3913,7 +3916,7 @@
         <v>1</v>
       </c>
       <c r="O53" s="1" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
     </row>
     <row r="54" spans="1:15" ht="136" x14ac:dyDescent="0.2">
@@ -3921,19 +3924,19 @@
         <v>53</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="D54" s="1">
         <v>2017</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="G54" s="1" t="s">
         <v>54</v>
@@ -3942,7 +3945,7 @@
         <v>55</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="K54" s="1" t="s">
         <v>41</v>
@@ -3954,7 +3957,7 @@
         <v>53</v>
       </c>
       <c r="O54" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
     </row>
     <row r="55" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -3962,10 +3965,10 @@
         <v>54</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D55" s="1">
         <v>2018</v>
@@ -3983,7 +3986,7 @@
         <v>21</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K55" s="1" t="s">
         <v>41</v>
@@ -3998,7 +4001,7 @@
         <v>36</v>
       </c>
       <c r="O55" s="1" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
     </row>
     <row r="56" spans="1:15" ht="85" x14ac:dyDescent="0.2">
@@ -4006,34 +4009,34 @@
         <v>55</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="D56" s="1">
         <v>2016</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="F56" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="J56" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="G56" s="1" t="s">
+      <c r="K56" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="H56" s="1" t="s">
-        <v>310</v>
-      </c>
-      <c r="J56" s="1" t="s">
-        <v>311</v>
-      </c>
-      <c r="K56" s="1" t="s">
-        <v>312</v>
-      </c>
       <c r="L56" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="M56" s="1" t="s">
         <v>23</v>
@@ -4042,7 +4045,7 @@
         <v>55</v>
       </c>
       <c r="O56" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="57" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -4050,10 +4053,10 @@
         <v>56</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D57" s="1">
         <v>2019</v>
@@ -4062,7 +4065,7 @@
         <v>3</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G57" s="1" t="s">
         <v>54</v>
@@ -4074,7 +4077,7 @@
         <v>41</v>
       </c>
       <c r="J57" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="K57" s="1" t="s">
         <v>41</v>
@@ -4089,7 +4092,7 @@
         <v>21</v>
       </c>
       <c r="O57" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
     </row>
     <row r="58" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -4097,34 +4100,34 @@
         <v>57</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D58" s="1">
         <v>2019</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H58" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I58" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="K58" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="M58" s="1" t="s">
         <v>23</v>
@@ -4133,7 +4136,7 @@
         <v>57</v>
       </c>
       <c r="O58" s="2" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
     </row>
     <row r="59" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -4141,28 +4144,28 @@
         <v>58</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="D59" s="1">
         <v>2017</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="L59" s="1" t="s">
         <v>22</v>
@@ -4171,10 +4174,10 @@
         <v>23</v>
       </c>
       <c r="N59" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="O59" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
     </row>
     <row r="60" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -4182,28 +4185,28 @@
         <v>59</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="D60" s="1">
         <v>2015</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="L60" s="1" t="s">
         <v>22</v>
@@ -4215,7 +4218,7 @@
         <v>59</v>
       </c>
       <c r="O60" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="61" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -4223,10 +4226,10 @@
         <v>60</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="D61" s="1">
         <v>2019</v>
@@ -4244,7 +4247,7 @@
         <v>21</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="K61" s="1" t="s">
         <v>41</v>
@@ -4259,7 +4262,7 @@
         <v>36</v>
       </c>
       <c r="O61" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
     </row>
     <row r="62" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -4267,10 +4270,10 @@
         <v>61</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="D62" s="1">
         <v>2019</v>
@@ -4303,7 +4306,7 @@
         <v>1</v>
       </c>
       <c r="O62" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
     </row>
     <row r="63" spans="1:15" ht="85" x14ac:dyDescent="0.2">
@@ -4311,31 +4314,31 @@
         <v>62</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="D63" s="1">
         <v>2019</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="F63" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="G63" s="1" t="s">
+        <v>343</v>
+      </c>
+      <c r="H63" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="J63" s="2" t="s">
         <v>345</v>
-      </c>
-      <c r="G63" s="1" t="s">
-        <v>346</v>
-      </c>
-      <c r="H63" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I63" s="1" t="s">
-        <v>347</v>
-      </c>
-      <c r="J63" s="2" t="s">
-        <v>348</v>
       </c>
       <c r="K63" s="1" t="s">
         <v>41</v>
@@ -4347,7 +4350,7 @@
         <v>62</v>
       </c>
       <c r="O63" s="2" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
     </row>
     <row r="64" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -4355,10 +4358,10 @@
         <v>63</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="D64" s="1">
         <v>2019</v>
@@ -4367,22 +4370,22 @@
         <v>5</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>55</v>
       </c>
       <c r="J64" s="1" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="K64" s="1" t="s">
         <v>41</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="M64" s="1" t="s">
         <v>23</v>
@@ -4391,7 +4394,7 @@
         <v>63</v>
       </c>
       <c r="O64" s="2" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
     </row>
     <row r="65" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -4399,28 +4402,28 @@
         <v>64</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="D65" s="1">
         <v>2019</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>371</v>
+        <v>368</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>372</v>
+        <v>369</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>55</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>373</v>
+        <v>370</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>41</v>
@@ -4432,7 +4435,7 @@
         <v>64</v>
       </c>
       <c r="O65" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
     </row>
     <row r="66" spans="1:15" ht="85" x14ac:dyDescent="0.2">
@@ -4440,40 +4443,40 @@
         <v>65</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="D66" s="1">
         <v>2019</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H66" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>41</v>
       </c>
       <c r="M66" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="N66" s="1">
         <v>65</v>
       </c>
       <c r="O66" s="1" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
     </row>
     <row r="67" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -4481,10 +4484,10 @@
         <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="D67" s="1">
         <v>2017</v>
@@ -4493,7 +4496,7 @@
         <v>3</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>20</v>
@@ -4502,10 +4505,10 @@
         <v>55</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="K67" s="1" t="s">
         <v>41</v>
@@ -4517,7 +4520,7 @@
         <v>66</v>
       </c>
       <c r="O67" s="2" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
     </row>
     <row r="68" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -4525,10 +4528,10 @@
         <v>67</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D68" s="1">
         <v>2013</v>
@@ -4537,25 +4540,25 @@
         <v>3</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="K68" s="1" t="s">
         <v>41</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="M68" s="1" t="s">
         <v>23</v>
@@ -4564,7 +4567,7 @@
         <v>67</v>
       </c>
       <c r="O68" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
     </row>
     <row r="69" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -4572,10 +4575,10 @@
         <v>68</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D69" s="1">
         <v>2018</v>
@@ -4587,13 +4590,13 @@
         <v>53</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="H69" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>41</v>
@@ -4605,10 +4608,10 @@
         <v>23</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="O69" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
     </row>
     <row r="70" spans="1:15" ht="85" x14ac:dyDescent="0.2">
@@ -4616,31 +4619,31 @@
         <v>69</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D70" s="1">
         <v>2018</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I70" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="J70" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>41</v>
@@ -4652,7 +4655,7 @@
         <v>69</v>
       </c>
       <c r="O70" s="2" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
     </row>
     <row r="71" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -4660,10 +4663,10 @@
         <v>70</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="D71" s="1">
         <v>2018</v>
@@ -4672,7 +4675,7 @@
         <v>3</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>20</v>
@@ -4687,7 +4690,7 @@
         <v>70</v>
       </c>
       <c r="O71" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
     </row>
     <row r="72" spans="1:15" ht="102" x14ac:dyDescent="0.2">
@@ -4695,10 +4698,10 @@
         <v>71</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>367</v>
+        <v>364</v>
       </c>
       <c r="D72" s="1">
         <v>2017</v>
@@ -4710,13 +4713,13 @@
         <v>53</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>21</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="M72" s="1" t="s">
         <v>23</v>
@@ -4725,7 +4728,7 @@
         <v>71</v>
       </c>
       <c r="O72" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix data source typo
</commit_message>
<xml_diff>
--- a/supplemental_data/data_sources_standardized.xlsx
+++ b/supplemental_data/data_sources_standardized.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Keith/Dev/research/johns-hopkins/dredze/mental-health-datasets/supplemental_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{200B73E1-9814-6E4C-9A89-590F04E628E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE857EEA-E3A5-914B-8EFB-28FEE7E5FD08}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="26060" windowHeight="11880" xr2:uid="{A1A2B0B9-EC2A-0C4B-9F85-EE07A9280363}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="26060" windowHeight="11880" xr2:uid="{A1A2B0B9-EC2A-0C4B-9F85-EE07A9280363}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1137,9 +1137,6 @@
     <t>https://www.aclweb.org/anthology/D19-6213/</t>
   </si>
   <si>
-    <t>death_row_last_statements, tumblr, the_kernel</t>
-  </si>
-  <si>
     <t>suicide_(ideation), imminent_death, depression, loneliness</t>
   </si>
   <si>
@@ -1225,6 +1222,9 @@
   </si>
   <si>
     <t>combined (253)</t>
+  </si>
+  <si>
+    <t>death_row_last_statements, tumblr, experience_project</t>
   </si>
 </sst>
 </file>
@@ -1592,8 +1592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48F7582B-A8CE-1545-B88D-1FB6E3E8BB38}">
   <dimension ref="A1:O72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G57" workbookViewId="0">
-      <selection activeCell="N59" sqref="N59"/>
+    <sheetView tabSelected="1" topLeftCell="A62" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="24.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1816,7 +1816,7 @@
         <v>43</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="M5" s="1" t="s">
         <v>23</v>
@@ -2024,7 +2024,7 @@
         <v>21</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>41</v>
@@ -2065,7 +2065,7 @@
         <v>21</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="K11" s="1" t="s">
         <v>41</v>
@@ -3162,7 +3162,7 @@
         <v>172</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="K36" s="1" t="s">
         <v>41</v>
@@ -4411,10 +4411,10 @@
         <v>2019</v>
       </c>
       <c r="E65" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="F65" s="1" t="s">
         <v>368</v>
-      </c>
-      <c r="F65" s="1" t="s">
-        <v>369</v>
       </c>
       <c r="G65" s="1" t="s">
         <v>343</v>
@@ -4423,7 +4423,7 @@
         <v>55</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="K65" s="1" t="s">
         <v>41</v>
@@ -4435,7 +4435,7 @@
         <v>64</v>
       </c>
       <c r="O65" s="2" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="66" spans="1:15" ht="85" x14ac:dyDescent="0.2">
@@ -4464,7 +4464,7 @@
         <v>21</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="K66" s="1" t="s">
         <v>41</v>
@@ -4476,7 +4476,7 @@
         <v>65</v>
       </c>
       <c r="O66" s="1" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="67" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -4505,10 +4505,10 @@
         <v>55</v>
       </c>
       <c r="I67" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="J67" s="1" t="s">
         <v>374</v>
-      </c>
-      <c r="J67" s="1" t="s">
-        <v>375</v>
       </c>
       <c r="K67" s="1" t="s">
         <v>41</v>
@@ -4520,7 +4520,7 @@
         <v>66</v>
       </c>
       <c r="O67" s="2" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="68" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -4543,16 +4543,16 @@
         <v>136</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I68" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="J68" s="1" t="s">
         <v>378</v>
-      </c>
-      <c r="J68" s="1" t="s">
-        <v>379</v>
       </c>
       <c r="K68" s="1" t="s">
         <v>41</v>
@@ -4567,7 +4567,7 @@
         <v>67</v>
       </c>
       <c r="O68" s="1" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="69" spans="1:15" ht="51" x14ac:dyDescent="0.2">
@@ -4590,13 +4590,13 @@
         <v>53</v>
       </c>
       <c r="G69" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I69" s="1" t="s">
         <v>381</v>
-      </c>
-      <c r="H69" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I69" s="1" t="s">
-        <v>382</v>
       </c>
       <c r="K69" s="1" t="s">
         <v>41</v>
@@ -4608,10 +4608,10 @@
         <v>23</v>
       </c>
       <c r="N69" s="1" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="O69" s="1" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="70" spans="1:15" ht="85" x14ac:dyDescent="0.2">
@@ -4628,22 +4628,22 @@
         <v>2018</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>365</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>55</v>
       </c>
       <c r="I70" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="J70" s="1" t="s">
         <v>387</v>
-      </c>
-      <c r="J70" s="1" t="s">
-        <v>388</v>
       </c>
       <c r="K70" s="1" t="s">
         <v>41</v>
@@ -4655,7 +4655,7 @@
         <v>69</v>
       </c>
       <c r="O70" s="2" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="71" spans="1:15" ht="68" x14ac:dyDescent="0.2">
@@ -4690,7 +4690,7 @@
         <v>70</v>
       </c>
       <c r="O71" s="1" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="72" spans="1:15" ht="102" x14ac:dyDescent="0.2">
@@ -4713,13 +4713,13 @@
         <v>53</v>
       </c>
       <c r="G72" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I72" s="1" t="s">
         <v>392</v>
-      </c>
-      <c r="H72" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I72" s="1" t="s">
-        <v>393</v>
       </c>
       <c r="M72" s="1" t="s">
         <v>23</v>
@@ -4728,7 +4728,7 @@
         <v>71</v>
       </c>
       <c r="O72" s="1" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
   </sheetData>

</xml_diff>